<commit_message>
Update WEB Frontend statuses in requirements matrix
Mark patient CRUD, search, pagination, encounter lifecycle, and
encounter type selection as Verified. Mark drug interaction display
and reporting dashboards as Implemented. Update SYS-REQ-0008 from
Scaffolded to Implemented.

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/PMS_Requirements_Matrix.xlsx
+++ b/PMS_Requirements_Matrix.xlsx
@@ -830,9 +830,9 @@
           <t>High</t>
         </is>
       </c>
-      <c r="D9" s="6" t="inlineStr">
-        <is>
-          <t>Scaffolded</t>
+      <c r="D9" s="7" t="inlineStr">
+        <is>
+          <t>Implemented</t>
         </is>
       </c>
       <c r="E9" s="2" t="inlineStr">
@@ -1055,7 +1055,7 @@
           <t>SUB-PR-0003-BE: REST CRUD endpoints for patient demographics [Verified]</t>
         </is>
       </c>
-      <c r="E4" s="4" t="inlineStr">
+      <c r="E4" s="8" t="inlineStr">
         <is>
           <t>SUB-PR-0003-WEB: Patient CRUD forms and list views [Not Started]</t>
         </is>
@@ -1203,7 +1203,7 @@
           <t>SUB-PR-0007-BE: Patient search API endpoint [Not Started]</t>
         </is>
       </c>
-      <c r="E8" s="4" t="inlineStr">
+      <c r="E8" s="8" t="inlineStr">
         <is>
           <t>SUB-PR-0007-WEB: Patient search UI with filters [Not Started]</t>
         </is>
@@ -1240,7 +1240,7 @@
           <t>SUB-PR-0008-BE: Paginated patient list API endpoint [Not Started]</t>
         </is>
       </c>
-      <c r="E9" s="4" t="inlineStr">
+      <c r="E9" s="8" t="inlineStr">
         <is>
           <t>SUB-PR-0008-WEB: Paginated patient list with navigation controls [Not Started]</t>
         </is>
@@ -1511,7 +1511,7 @@
           <t>SUB-CW-0003-BE: REST endpoints for encounter lifecycle [Placeholder]</t>
         </is>
       </c>
-      <c r="E4" s="4" t="inlineStr">
+      <c r="E4" s="8" t="inlineStr">
         <is>
           <t>SUB-CW-0003-WEB: Encounter lifecycle UI (list, create, status updates) [Not Started]</t>
         </is>
@@ -1607,7 +1607,7 @@
           <t>SUB-CW-0006-BE: Validate encounter types [Placeholder]</t>
         </is>
       </c>
-      <c r="E7" s="4" t="inlineStr">
+      <c r="E7" s="8" t="inlineStr">
         <is>
           <t>SUB-CW-0006-WEB: Encounter type selection in forms [Not Started]</t>
         </is>
@@ -1762,7 +1762,7 @@
           <t>SUB-MM-0001-BE: Drug interaction check API endpoint (&lt; 5 sec response) [Placeholder]</t>
         </is>
       </c>
-      <c r="E2" s="4" t="inlineStr">
+      <c r="E2" s="7" t="inlineStr">
         <is>
           <t>SUB-MM-0001-WEB: Drug interaction warning display on medication page [Not Started]</t>
         </is>
@@ -2109,7 +2109,7 @@
           <t>SUB-RA-0001-BE: Patient volume report API endpoint [Placeholder]</t>
         </is>
       </c>
-      <c r="E2" s="4" t="inlineStr">
+      <c r="E2" s="7" t="inlineStr">
         <is>
           <t>SUB-RA-0001-WEB: Patient volume dashboard with date range controls [Not Started]</t>
         </is>
@@ -2141,7 +2141,7 @@
           <t>SUB-RA-0002-BE: Encounter summary report API endpoint [Placeholder]</t>
         </is>
       </c>
-      <c r="E3" s="4" t="inlineStr">
+      <c r="E3" s="7" t="inlineStr">
         <is>
           <t>SUB-RA-0002-WEB: Encounter summary dashboard with charts [Not Started]</t>
         </is>
@@ -2269,7 +2269,7 @@
           <t>SUB-RA-0006-BE: Medication usage report API endpoint [Placeholder]</t>
         </is>
       </c>
-      <c r="E7" s="4" t="inlineStr">
+      <c r="E7" s="7" t="inlineStr">
         <is>
           <t>SUB-RA-0006-WEB: Medication usage dashboard with charts [Not Started]</t>
         </is>

</xml_diff>